<commit_message>
add functionality for portfolio calculations
</commit_message>
<xml_diff>
--- a/files/transactions.xlsx
+++ b/files/transactions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/21f3278d21428556/Documents/Software/Python/Finance/IEX/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnk\Desktop\github\IEX\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="131" documentId="11_FFC65FC042496CEC7D1E2B2B5429AEAE4A1E5730" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1CDD7CF6-67C4-449A-9A14-F4352192FE05}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC02E516-A8E2-4621-A7C2-B0508D7733A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="83" windowWidth="22485" windowHeight="14317" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15" yWindow="83" windowWidth="22485" windowHeight="14317" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t>date</t>
   </si>
@@ -82,6 +82,12 @@
   </si>
   <si>
     <t>GTLB</t>
+  </si>
+  <si>
+    <t>cost</t>
+  </si>
+  <si>
+    <t>Sell</t>
   </si>
 </sst>
 </file>
@@ -484,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -499,7 +505,7 @@
     <col min="5" max="5" width="7.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -515,8 +521,11 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="2">
         <v>44074</v>
       </c>
@@ -532,8 +541,12 @@
       <c r="E2">
         <v>325.10000000000002</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F2">
+        <f>D2*E2</f>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="2">
         <v>44222</v>
       </c>
@@ -549,8 +562,12 @@
       <c r="E3">
         <v>19.57</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F3">
+        <f t="shared" ref="F3:F12" si="0">D3*E3</f>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="2">
         <v>44253</v>
       </c>
@@ -566,8 +583,12 @@
       <c r="E4">
         <v>94.91</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>1999.9999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="2">
         <v>44354</v>
       </c>
@@ -583,8 +604,12 @@
       <c r="E5">
         <v>32.159999999999997</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="2">
         <v>44378</v>
       </c>
@@ -595,13 +620,17 @@
         <v>6</v>
       </c>
       <c r="D6">
-        <v>21.433929911049191</v>
+        <v>21</v>
       </c>
       <c r="E6">
         <v>93.31</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>1959.51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="2">
         <v>44378</v>
       </c>
@@ -617,8 +646,12 @@
       <c r="E7">
         <v>80.11</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="2">
         <v>44405</v>
       </c>
@@ -634,8 +667,12 @@
       <c r="E8">
         <v>32.56</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="2">
         <v>44413</v>
       </c>
@@ -651,8 +688,12 @@
       <c r="E9">
         <v>22.52</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>2000.0000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="2">
         <v>44473</v>
       </c>
@@ -668,8 +709,12 @@
       <c r="E10">
         <v>24.14</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>1999.9999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="2">
         <v>44480</v>
       </c>
@@ -685,8 +730,12 @@
       <c r="E11">
         <v>206.95</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="2">
         <v>44487</v>
       </c>
@@ -701,6 +750,31 @@
       </c>
       <c r="E12">
         <v>110</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>2000.0000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13" s="2">
+        <v>44659</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13">
+        <v>-21</v>
+      </c>
+      <c r="E13">
+        <v>101</v>
+      </c>
+      <c r="F13">
+        <f t="shared" ref="F13" si="1">D13*E13</f>
+        <v>-2121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
replace the portfolio function with enhanced function which includes class
</commit_message>
<xml_diff>
--- a/files/transactions.xlsx
+++ b/files/transactions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnk\Desktop\github\IEX\tests\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnk\Desktop\github\IEX\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72F62463-D3C6-4DD4-BEAC-A59316DCC413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55CAFB91-B9A3-4240-9B63-2C68E7C69647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15" yWindow="1837" windowWidth="22485" windowHeight="11866" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
   <si>
     <t>date</t>
   </si>
@@ -85,12 +85,6 @@
   </si>
   <si>
     <t>cost</t>
-  </si>
-  <si>
-    <t>Sell</t>
-  </si>
-  <si>
-    <t>BLKRK</t>
   </si>
 </sst>
 </file>
@@ -493,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+      <selection activeCell="A13" sqref="A13:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -760,174 +754,6 @@
         <v>2000.0000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A13" s="2">
-        <v>44659</v>
-      </c>
-      <c r="B13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13">
-        <v>-15</v>
-      </c>
-      <c r="E13">
-        <v>101</v>
-      </c>
-      <c r="F13">
-        <f t="shared" ref="F13" si="1">D13*E13</f>
-        <v>-1515</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A14" s="2">
-        <v>44665</v>
-      </c>
-      <c r="B14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14">
-        <v>10</v>
-      </c>
-      <c r="E14">
-        <v>95</v>
-      </c>
-      <c r="F14">
-        <f t="shared" ref="F14" si="2">D14*E14</f>
-        <v>950</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A15" s="2">
-        <v>44673</v>
-      </c>
-      <c r="B15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15">
-        <v>-5</v>
-      </c>
-      <c r="E15">
-        <v>101</v>
-      </c>
-      <c r="F15">
-        <f t="shared" ref="F15:F17" si="3">D15*E15</f>
-        <v>-505</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A16" s="2">
-        <v>44680</v>
-      </c>
-      <c r="B16" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16">
-        <v>5</v>
-      </c>
-      <c r="E16">
-        <v>110</v>
-      </c>
-      <c r="F16">
-        <f t="shared" si="3"/>
-        <v>550</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A17" s="2">
-        <v>44687</v>
-      </c>
-      <c r="B17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17">
-        <v>-62</v>
-      </c>
-      <c r="E17">
-        <v>50</v>
-      </c>
-      <c r="F17">
-        <f t="shared" si="3"/>
-        <v>-3100</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A18" s="2">
-        <v>44691</v>
-      </c>
-      <c r="B18" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18">
-        <v>5</v>
-      </c>
-      <c r="E18">
-        <v>10</v>
-      </c>
-      <c r="F18">
-        <f t="shared" ref="F18:F19" si="4">D18*E18</f>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A19" s="2">
-        <v>44693</v>
-      </c>
-      <c r="B19" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D19">
-        <v>5</v>
-      </c>
-      <c r="E19">
-        <v>12</v>
-      </c>
-      <c r="F19">
-        <f t="shared" si="4"/>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A20" s="2">
-        <v>44697</v>
-      </c>
-      <c r="B20" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" t="s">
-        <v>19</v>
-      </c>
-      <c r="D20">
-        <v>5</v>
-      </c>
-      <c r="E20">
-        <v>14</v>
-      </c>
-      <c r="F20">
-        <f t="shared" ref="F20" si="5">D20*E20</f>
-        <v>70</v>
-      </c>
-    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E9">
     <sortCondition ref="A1:A9"/>

</xml_diff>

<commit_message>
add transaction checks, single day fix, unit testing update
</commit_message>
<xml_diff>
--- a/files/transactions.xlsx
+++ b/files/transactions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnk\Desktop\github\IEX\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C26D1B6-6747-4EBB-B613-40BB205601A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{467CA46B-BCA5-47BF-A692-BEE67CF2B2FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="368" windowWidth="22485" windowHeight="11865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -45,9 +45,6 @@
     <t>price</t>
   </si>
   <si>
-    <t>Buy</t>
-  </si>
-  <si>
     <t>ZM</t>
   </si>
   <si>
@@ -85,6 +82,9 @@
   </si>
   <si>
     <t>cost</t>
+  </si>
+  <si>
+    <t>BUY</t>
   </si>
 </sst>
 </file>
@@ -490,7 +490,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -514,13 +514,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
@@ -528,10 +528,10 @@
         <v>44074</v>
       </c>
       <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
       </c>
       <c r="D2">
         <v>6.1519532451553367</v>
@@ -548,10 +548,10 @@
         <v>44222</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3">
         <v>102.19724067450178</v>
@@ -568,10 +568,10 @@
         <v>44253</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4">
         <v>21.072595090085343</v>
@@ -588,10 +588,10 @@
         <v>44354</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5">
         <v>62</v>
@@ -608,10 +608,10 @@
         <v>44378</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D6">
         <v>21</v>
@@ -628,10 +628,10 @@
         <v>44378</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D7">
         <v>24.965672200724004</v>
@@ -648,10 +648,10 @@
         <v>44405</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D8">
         <v>61.425061425061422</v>
@@ -668,10 +668,10 @@
         <v>44413</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D9">
         <v>88.80994671403198</v>
@@ -688,10 +688,10 @@
         <v>44473</v>
       </c>
       <c r="B10" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D10">
         <v>82.850041425020706</v>
@@ -708,10 +708,10 @@
         <v>44480</v>
       </c>
       <c r="B11" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D11">
         <v>9.6641700893935738</v>
@@ -728,10 +728,10 @@
         <v>44487</v>
       </c>
       <c r="B12" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D12">
         <v>18.181818181818183</v>

</xml_diff>